<commit_message>
More progress on the description paper.
</commit_message>
<xml_diff>
--- a/inputs/metadata_configuration_file.xlsx
+++ b/inputs/metadata_configuration_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\repositories\data-analysis\iotc-tcac-simulations\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09A6ACA-9401-4CC6-BBFF-F517176586A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34987A11-31B9-4FE2-8308-9B8C7CE1E31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{285539CB-9A0C-4AA0-B324-24EFEBF5A269}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{285539CB-9A0C-4AA0-B324-24EFEBF5A269}"/>
   </bookViews>
   <sheets>
     <sheet name="CPC" sheetId="1" r:id="rId1"/>
@@ -336,9 +336,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -348,6 +345,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -686,7 +686,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,8 +813,8 @@
       <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="3">
-        <v>1.49E-2</v>
+      <c r="C11" s="7">
+        <v>1.49</v>
       </c>
     </row>
   </sheetData>
@@ -855,7 +855,7 @@
       <c r="B2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -866,7 +866,7 @@
       <c r="B3" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -877,7 +877,7 @@
       <c r="B4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -888,7 +888,7 @@
       <c r="B5" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -899,7 +899,7 @@
       <c r="B6" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -910,7 +910,7 @@
       <c r="B7" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -921,7 +921,7 @@
       <c r="B8" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -932,7 +932,7 @@
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -943,7 +943,7 @@
       <c r="B10" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -954,7 +954,7 @@
       <c r="B11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -965,7 +965,7 @@
       <c r="B12" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>51</v>
       </c>
     </row>
@@ -976,12 +976,12 @@
       <c r="B13" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14" s="4"/>
+      <c r="C14" s="3"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
@@ -999,29 +999,29 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="82.42578125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="57" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="31.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="82.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="57" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1032,7 +1032,7 @@
       <c r="B2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>1995</v>
       </c>
       <c r="D2" s="1"/>
@@ -1044,7 +1044,7 @@
       <c r="B3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D3" s="1"/>
@@ -1056,7 +1056,7 @@
       <c r="B4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>82</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1070,7 +1070,7 @@
       <c r="B5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>69</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1084,7 +1084,7 @@
       <c r="B6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>70</v>
       </c>
       <c r="D6" s="1"/>
@@ -1096,7 +1096,7 @@
       <c r="B7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1110,7 +1110,7 @@
       <c r="B8" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>72</v>
       </c>
       <c r="D8" s="1"/>
@@ -1122,7 +1122,7 @@
       <c r="B9" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>73</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1136,13 +1136,13 @@
       <c r="B10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>5200</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="7"/>
+      <c r="C11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finalisation of simulation tool description
</commit_message>
<xml_diff>
--- a/inputs/metadata_configuration_file.xlsx
+++ b/inputs/metadata_configuration_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\repositories\data-analysis\iotc-tcac-simulations\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34987A11-31B9-4FE2-8308-9B8C7CE1E31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5F7254-6BB0-4B25-BBCA-085D1F0F5781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{285539CB-9A0C-4AA0-B324-24EFEBF5A269}"/>
   </bookViews>
@@ -289,10 +289,10 @@
     <t>EUR</t>
   </si>
   <si>
-    <t>Flag state of the fishery vessels, combining the CPC in the case of European Union Member States and aggregating all non-CPCs as others (OTH) or not elsewehere included (NEI)</t>
-  </si>
-  <si>
     <t>Similar to flag code except in the case of European Union countries (EUR)</t>
+  </si>
+  <si>
+    <t>Flag state of the fishery vessels, combining the CPC in the case of European Union Member States and aggregating all non-CPCs as others (OTH) or not elsewhere included (NEI)</t>
   </si>
 </sst>
 </file>
@@ -999,7 +999,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,7 +1007,7 @@
     <col min="1" max="1" width="31.42578125" style="5" customWidth="1"/>
     <col min="2" max="2" width="82.42578125" style="5" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="57" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.42578125" style="5" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
@@ -1042,7 +1042,7 @@
         <v>56</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>65</v>
@@ -1054,7 +1054,7 @@
         <v>57</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>82</v>

</xml_diff>